<commit_message>
StaticDataAPIs Creations and Adding API versions attributes
</commit_message>
<xml_diff>
--- a/src/test/java/Static_Data/Data/Static_Data.xlsx
+++ b/src/test/java/Static_Data/Data/Static_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajmal.syed.LOGICIELSERVICE\eclipse-workspace\OMS_API\src\test\java\Static_Data_V3\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation_OMSAPI\src\test\java\Static_Data\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0A25D4-1F06-40AC-ADD1-45B1939B4A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F92AF0-8124-42C3-800E-EFFAA2CC9AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="326" xr2:uid="{A77A0332-03F7-4C79-B0EA-4DB171BB1F0C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="326" xr2:uid="{A77A0332-03F7-4C79-B0EA-4DB171BB1F0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="9" r:id="rId1"/>
@@ -27,6 +27,11 @@
     <sheet name="ETBHTB" sheetId="22" r:id="rId12"/>
     <sheet name="BlotterPackagePermissions" sheetId="20" r:id="rId13"/>
     <sheet name="BlotterPermissions" sheetId="21" r:id="rId14"/>
+    <sheet name="PutCall" sheetId="23" r:id="rId15"/>
+    <sheet name="CoveredUncovered" sheetId="24" r:id="rId16"/>
+    <sheet name="CustomerFirm" sheetId="25" r:id="rId17"/>
+    <sheet name="OptionOrderType" sheetId="26" r:id="rId18"/>
+    <sheet name="OptionTIF" sheetId="27" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="285">
   <si>
     <t>Content_Type</t>
   </si>
@@ -754,6 +759,156 @@
   </si>
   <si>
     <t>Verify_StaticData_BlotterPermissions_TC0001</t>
+  </si>
+  <si>
+    <t>/int/ord/api/v3/staticData/PutCall</t>
+  </si>
+  <si>
+    <t>Verify_StaticData_PutCall_TC0001</t>
+  </si>
+  <si>
+    <t>Verify_StaticData_PutCall_TC0002</t>
+  </si>
+  <si>
+    <t>CALL</t>
+  </si>
+  <si>
+    <t>StaticData_PutCall_BasePath</t>
+  </si>
+  <si>
+    <t>StaticData_PutCall_StatusCode</t>
+  </si>
+  <si>
+    <t>Validate_PutCall_Name</t>
+  </si>
+  <si>
+    <t>Validate_PutCall_Value</t>
+  </si>
+  <si>
+    <t>StaticData_PutCall_TestCases</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>Verify_StaticData_CoveredUncovered_TC0001</t>
+  </si>
+  <si>
+    <t>StaticData_CoveredUncovered_TestCases</t>
+  </si>
+  <si>
+    <t>StaticData_CoveredUncovered_BasePath</t>
+  </si>
+  <si>
+    <t>StaticData_CoveredUncovered_StatusCode</t>
+  </si>
+  <si>
+    <t>Validate_CoveredUncovered_Name</t>
+  </si>
+  <si>
+    <t>Validate_CoveredUncovered_Value</t>
+  </si>
+  <si>
+    <t>/int/ord/api/v3/staticData/CoveredUncovered</t>
+  </si>
+  <si>
+    <t>Verify_StaticData_CoveredUncovered_TC0002</t>
+  </si>
+  <si>
+    <t>COVERED</t>
+  </si>
+  <si>
+    <t>UNCOVERED</t>
+  </si>
+  <si>
+    <t>StaticData_CustomerFirm_TestCases</t>
+  </si>
+  <si>
+    <t>StaticData_CustomerFirm_BasePath</t>
+  </si>
+  <si>
+    <t>StaticData_CustomerFirm_StatusCode</t>
+  </si>
+  <si>
+    <t>Validate_CustomerFirm_Name</t>
+  </si>
+  <si>
+    <t>Validate_CustomerFirm_Value</t>
+  </si>
+  <si>
+    <t>Verify_StaticData_CustomerFirm_TC0001</t>
+  </si>
+  <si>
+    <t>/int/ord/api/v3/staticData/CustomerFirm</t>
+  </si>
+  <si>
+    <t>Verify_StaticData_CustomerFirm_TC0002</t>
+  </si>
+  <si>
+    <t>FIRM</t>
+  </si>
+  <si>
+    <t>CUSTOMER</t>
+  </si>
+  <si>
+    <t>Verify_StaticData_OptionOrderType_TC0001</t>
+  </si>
+  <si>
+    <t>/int/ord/api/v3/staticData/OptionOrderType</t>
+  </si>
+  <si>
+    <t>Verify_StaticData_OptionOrderType_TC0002</t>
+  </si>
+  <si>
+    <t>StaticData_OptionOrderType_TestCases</t>
+  </si>
+  <si>
+    <t>StaticData_OptionOrderType_BasePath</t>
+  </si>
+  <si>
+    <t>StaticData_OptionOrderType_StatusCode</t>
+  </si>
+  <si>
+    <t>Validate_OptionOrderType_Name</t>
+  </si>
+  <si>
+    <t>Validate_OptionOrderType_Value</t>
+  </si>
+  <si>
+    <t>StaticData_OptionTIF_TestCases</t>
+  </si>
+  <si>
+    <t>StaticData_OptionTIF_BasePath</t>
+  </si>
+  <si>
+    <t>StaticData_OptionTIF_StatusCode</t>
+  </si>
+  <si>
+    <t>Validate_OptionTIF_Name</t>
+  </si>
+  <si>
+    <t>Validate_OptionTIF_Value</t>
+  </si>
+  <si>
+    <t>Verify_StaticData_OptionTIF_TC0001</t>
+  </si>
+  <si>
+    <t>/int/ord/api/v3/staticData/OptionTIF</t>
+  </si>
+  <si>
+    <t>Verify_StaticData_OptionTIF_TC0002</t>
+  </si>
+  <si>
+    <t>DAY</t>
+  </si>
+  <si>
+    <t>Verify_StaticData_OptionTIF_TC0003</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>EndpointVersion</t>
   </si>
 </sst>
 </file>
@@ -1187,204 +1342,228 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F97819-0497-470B-932D-7124C01F5F73}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" customWidth="1"/>
-    <col min="7" max="7" width="34.7109375" customWidth="1"/>
+    <col min="1" max="2" width="35" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" customWidth="1"/>
+    <col min="8" max="8" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>176</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
-        <v>200</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>10001</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>177</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>10002</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>178</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>200</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>200</v>
+      </c>
+      <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>10003</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>179</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <v>200</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>200</v>
+      </c>
+      <c r="F5" t="s">
         <v>12</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>10004</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>180</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
-        <v>200</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>200</v>
+      </c>
+      <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>10005</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>181</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4">
-        <v>200</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>200</v>
+      </c>
+      <c r="F7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>182</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4">
-        <v>200</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>200</v>
+      </c>
+      <c r="F8" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1397,136 +1576,152 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6A00EB-9916-402E-A52E-47847770BA71}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B1" sqref="B1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" customWidth="1"/>
-    <col min="5" max="5" width="47.5703125" customWidth="1"/>
-    <col min="6" max="6" width="37.140625" customWidth="1"/>
-    <col min="7" max="7" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" customWidth="1"/>
+    <col min="6" max="6" width="47.5703125" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" customWidth="1"/>
+    <col min="8" max="8" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>217</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
-        <v>200</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
         <v>101</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>156</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>218</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
         <v>102</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>157</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>219</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>200</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>200</v>
+      </c>
+      <c r="F4" t="s">
         <v>103</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>158</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>220</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <v>200</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>200</v>
+      </c>
+      <c r="F5" t="s">
         <v>104</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>159</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>6</v>
+      <c r="H5" s="15" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1538,205 +1733,229 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19004EE8-B1F1-4529-B662-24C899BA3C5C}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B1" sqref="B1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.7109375" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.140625" customWidth="1"/>
-    <col min="7" max="7" width="34.7109375" customWidth="1"/>
+    <col min="1" max="2" width="51.7109375" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" customWidth="1"/>
+    <col min="8" max="8" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>221</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
-        <v>200</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
         <v>110</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>117</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>222</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
         <v>111</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>118</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>223</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>200</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>200</v>
+      </c>
+      <c r="F4" t="s">
         <v>112</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>119</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>224</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <v>200</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>200</v>
+      </c>
+      <c r="F5" t="s">
         <v>113</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>120</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>225</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
-        <v>200</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>200</v>
+      </c>
+      <c r="F6" t="s">
         <v>114</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>121</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>226</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4">
-        <v>200</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>200</v>
+      </c>
+      <c r="F7" t="s">
         <v>115</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>122</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>227</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4">
-        <v>200</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>200</v>
+      </c>
+      <c r="F8" t="s">
         <v>116</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>123</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>6</v>
+      <c r="H8" s="8" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1748,80 +1967,87 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB0CA8EC-C674-4DE4-8CE4-3B36CC901C3B}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="69.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>173</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>228</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
-        <v>200</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>200</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1834,215 +2060,233 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49457023-34CD-4B1B-B7DC-20BBA5A807F9}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B1" sqref="B1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.28515625" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="55.85546875" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.28515625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="35.28515625" customWidth="1"/>
-    <col min="8" max="8" width="39" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="63.28515625" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="55.85546875" customWidth="1"/>
+    <col min="6" max="6" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.28515625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="35.28515625" customWidth="1"/>
+    <col min="9" max="9" width="39" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>229</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
-        <v>200</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
         <v>134</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>1000</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>132</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>133</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>230</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
         <v>134</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>1000</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>138</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>133</v>
       </c>
       <c r="J3" s="10" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>231</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>200</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>200</v>
+      </c>
+      <c r="F4" t="s">
         <v>134</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1000</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>139</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>133</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>232</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <v>200</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>200</v>
+      </c>
+      <c r="F5" t="s">
         <v>134</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>1000</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>140</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>133</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>233</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
-        <v>200</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>200</v>
+      </c>
+      <c r="F6" t="s">
         <v>130</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="G6" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6" t="s">
-        <v>32</v>
+      <c r="H6">
+        <v>1</v>
       </c>
       <c r="I6" t="s">
         <v>32</v>
       </c>
       <c r="J6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2055,70 +2299,624 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6726326-2C70-4439-A0BF-1A27192F1C12}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" customWidth="1"/>
-    <col min="5" max="5" width="39" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" customWidth="1"/>
+    <col min="6" max="6" width="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>234</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
-        <v>200</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
         <v>132</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>133</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>133</v>
       </c>
+      <c r="H2" s="10" t="s">
+        <v>133</v>
+      </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81768D37-C102-4CB6-B153-7090BE3D93AD}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" customWidth="1"/>
+    <col min="8" max="8" width="34.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
+        <v>238</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
+        <v>244</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE88B395-5588-4CAE-91B8-7344D7D4DCBF}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" customWidth="1"/>
+    <col min="8" max="8" width="34.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
+        <v>253</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
+        <v>254</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC773AF-692E-4D32-B04F-4CD8F723C684}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" customWidth="1"/>
+    <col min="8" max="8" width="34.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
+        <v>263</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
+        <v>264</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBE75A1-59F4-4EE0-A196-5F3004F5BDCF}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" customWidth="1"/>
+    <col min="8" max="8" width="34.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C4F6CCF-BB7D-4457-B17E-E5A4145A94D1}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" customWidth="1"/>
+    <col min="8" max="8" width="34.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
+        <v>281</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>200</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -2126,203 +2924,225 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1319A557-D53B-4CAE-8A5D-C1F0018C299F}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
-    <col min="6" max="6" width="37.140625" customWidth="1"/>
-    <col min="7" max="7" width="37.140625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="34.7109375" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" customWidth="1"/>
+    <col min="8" max="8" width="37.140625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
-        <v>200</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>184</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>185</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>200</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>200</v>
+      </c>
+      <c r="F4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="H4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>186</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <v>200</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>200</v>
+      </c>
+      <c r="F5" t="s">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="I5" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>187</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
-        <v>200</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>200</v>
+      </c>
+      <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="9">
+      <c r="H6" s="9">
         <v>10001</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="I6" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>188</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4">
-        <v>200</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>200</v>
+      </c>
+      <c r="F7" t="s">
         <v>30</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2335,99 +3155,109 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A5A6CE-1FF1-41EB-A637-FC236B4E00FB}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.5703125" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" customWidth="1"/>
-    <col min="5" max="5" width="39" customWidth="1"/>
-    <col min="6" max="6" width="37.140625" customWidth="1"/>
-    <col min="7" max="7" width="41.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.7109375" customWidth="1"/>
+    <col min="1" max="1" width="46" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" customWidth="1"/>
+    <col min="6" max="6" width="39" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" customWidth="1"/>
+    <col min="8" max="8" width="41.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>189</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
-        <v>200</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
         <v>44</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>190</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
         <v>43</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2440,205 +3270,229 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7750D010-10D0-4EB3-A3FE-203D0C24AABA}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B1" sqref="B1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.140625" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" customWidth="1"/>
-    <col min="6" max="6" width="43" customWidth="1"/>
-    <col min="7" max="7" width="34.7109375" customWidth="1"/>
+    <col min="1" max="2" width="47.140625" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" customWidth="1"/>
+    <col min="6" max="6" width="43.42578125" customWidth="1"/>
+    <col min="7" max="7" width="43" customWidth="1"/>
+    <col min="8" max="8" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>191</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
-        <v>200</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
         <v>50</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
         <v>51</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>200</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>200</v>
+      </c>
+      <c r="F4" t="s">
         <v>44</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <v>200</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>200</v>
+      </c>
+      <c r="F5" t="s">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>195</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
-        <v>200</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>200</v>
+      </c>
+      <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>196</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4">
-        <v>200</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>200</v>
+      </c>
+      <c r="F7" t="s">
         <v>30</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>197</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4">
-        <v>200</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>200</v>
+      </c>
+      <c r="F8" t="s">
         <v>52</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>6</v>
+      <c r="H8" s="8" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2650,113 +3504,126 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8DFC57-1736-45E9-A86D-2443AC6C695A}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.28515625" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
-    <col min="6" max="6" width="37.140625" customWidth="1"/>
-    <col min="7" max="7" width="34.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="2" width="53.28515625" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" customWidth="1"/>
+    <col min="8" max="8" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>198</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
-        <v>200</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
         <v>57</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>199</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
         <v>58</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>2</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>200</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>200</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>200</v>
+      </c>
+      <c r="F4" t="s">
         <v>59</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>5</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>6</v>
+      <c r="H4" s="8" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2768,205 +3635,230 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552CD2B4-F7F5-4A73-BB5A-E209C9D92C70}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
-    <col min="6" max="6" width="37.140625" customWidth="1"/>
-    <col min="7" max="7" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" customWidth="1"/>
+    <col min="8" max="8" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>201</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
-        <v>200</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
         <v>69</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>202</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
         <v>70</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>203</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>200</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>200</v>
+      </c>
+      <c r="F4" t="s">
         <v>71</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>2</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>204</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <v>200</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>200</v>
+      </c>
+      <c r="F5" t="s">
         <v>72</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>3</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>205</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
-        <v>200</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>200</v>
+      </c>
+      <c r="F6" t="s">
         <v>73</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>4</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>206</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4">
-        <v>200</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>200</v>
+      </c>
+      <c r="F7" t="s">
         <v>74</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>5</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>207</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4">
-        <v>200</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>200</v>
+      </c>
+      <c r="F8" t="s">
         <v>75</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>6</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>6</v>
+      <c r="H8" s="8" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2978,113 +3870,125 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C633D2-212A-469D-B16A-DA7E2E5F6C2C}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B1" sqref="B1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="10" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="37.140625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="34.7109375" style="10" customWidth="1"/>
+    <col min="1" max="2" width="43" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="34.7109375" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>208</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3">
-        <v>200</v>
-      </c>
-      <c r="E2" s="10" t="s">
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>200</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="F2" s="10">
-        <v>1</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="10">
+        <v>1</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>209</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3">
-        <v>200</v>
-      </c>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>200</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="10">
+      <c r="G3" s="10">
         <v>2</v>
       </c>
-      <c r="G3" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>210</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
-        <v>200</v>
-      </c>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>200</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="10">
+      <c r="G4" s="10">
         <v>3</v>
       </c>
-      <c r="G4" s="15" t="s">
-        <v>6</v>
+      <c r="H4" s="15" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3096,136 +4000,152 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDDE52E5-B96A-42BA-9C18-471F7BF48EC7}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="10" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="37.140625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="34.7109375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="34.7109375" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>211</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3">
-        <v>200</v>
-      </c>
-      <c r="E2" s="10" t="s">
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>200</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="10">
-        <v>1</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="10">
+        <v>1</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>212</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3">
-        <v>200</v>
-      </c>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>200</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="10">
+      <c r="G3" s="10">
         <v>2</v>
       </c>
-      <c r="G3" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>213</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
-        <v>200</v>
-      </c>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>200</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="10">
+      <c r="G4" s="10">
         <v>3</v>
       </c>
-      <c r="G4" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>214</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3">
-        <v>200</v>
-      </c>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>200</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="F5" s="10">
+      <c r="G5" s="10">
         <v>4</v>
       </c>
-      <c r="G5" s="15" t="s">
-        <v>6</v>
+      <c r="H5" s="15" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3237,90 +4157,100 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A187E8-21EB-411C-ABE1-3FE3637DF611}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
-    <col min="6" max="6" width="37.140625" customWidth="1"/>
-    <col min="7" max="7" width="34.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" customWidth="1"/>
+    <col min="8" max="8" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>215</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
-        <v>200</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
         <v>72</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>3</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>216</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
         <v>73</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>4</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>6</v>
+      <c r="H3" s="15" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>